<commit_message>
tambahan kaos 30 set
</commit_message>
<xml_diff>
--- a/Kaos/REKAPITULASI.xlsx
+++ b/Kaos/REKAPITULASI.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mapan\progress\Kaos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56250235-2D2E-44EA-9CAC-F7114118FB9E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1870B2B-7BC6-4332-A07B-B33440463AF8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5925" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
   <si>
     <t>NO</t>
   </si>
@@ -82,6 +83,9 @@
   </si>
   <si>
     <t>FAKTUR</t>
+  </si>
+  <si>
+    <t>24 MARET 2021</t>
   </si>
 </sst>
 </file>
@@ -128,9 +132,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma [0]" xfId="1" builtinId="6"/>
@@ -412,20 +417,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L14"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -448,7 +457,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -461,147 +470,240 @@
       <c r="D2">
         <v>120</v>
       </c>
-      <c r="I2" t="s">
-        <v>11</v>
-      </c>
-      <c r="J2" t="s">
-        <v>12</v>
-      </c>
-      <c r="K2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>6</v>
       </c>
       <c r="D3">
         <v>120</v>
       </c>
-      <c r="I3" t="s">
-        <v>7</v>
-      </c>
-      <c r="J3">
-        <v>155000</v>
-      </c>
-      <c r="K3">
-        <v>215000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>8</v>
       </c>
       <c r="D4">
         <v>120</v>
       </c>
-      <c r="I4" t="s">
-        <v>6</v>
-      </c>
-      <c r="J4">
-        <v>60000</v>
-      </c>
-      <c r="K4">
-        <v>85000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
         <v>18</v>
       </c>
-      <c r="E5">
-        <v>110</v>
-      </c>
-      <c r="F5" s="1">
-        <f>D2-E5</f>
-        <v>10</v>
-      </c>
-      <c r="I5" t="s">
-        <v>8</v>
-      </c>
-      <c r="J5">
-        <v>40000</v>
-      </c>
-      <c r="K5">
-        <v>55000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E6">
         <v>110</v>
       </c>
       <c r="F6" s="1">
-        <f>D3-E6</f>
+        <f>D2-E6</f>
         <v>10</v>
       </c>
-      <c r="J6">
-        <f>SUM(J3:J5)</f>
-        <v>255000</v>
-      </c>
-      <c r="K6">
-        <f>SUM(K3:K5)</f>
-        <v>355000</v>
-      </c>
-      <c r="L6">
-        <f>K6-J6</f>
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E7">
         <v>110</v>
       </c>
       <c r="F7" s="1">
-        <f>D4-E7</f>
+        <f>D3-E7</f>
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="J9" s="1">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <v>110</v>
+      </c>
+      <c r="F8" s="1">
+        <f>D4-E8</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10" s="2">
+        <v>44287</v>
+      </c>
+      <c r="C10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10">
+        <v>30</v>
+      </c>
+      <c r="F10" s="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11">
+        <v>30</v>
+      </c>
+      <c r="F11" s="1">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C801C50D-43EE-4BA0-99C5-093CD08C00D4}">
+  <dimension ref="B2:E15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K27" sqref="K27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1">
+        <v>155000</v>
+      </c>
+      <c r="D3" s="1">
+        <v>220000</v>
+      </c>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="1">
+        <v>60000</v>
+      </c>
+      <c r="D4" s="1">
+        <v>85000</v>
+      </c>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="1">
+        <v>40000</v>
+      </c>
+      <c r="D5" s="1">
+        <v>55000</v>
+      </c>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C6" s="1">
+        <f>SUM(C3:C5)</f>
+        <v>255000</v>
+      </c>
+      <c r="D6" s="1">
+        <f>SUM(D3:D5)</f>
+        <v>360000</v>
+      </c>
+      <c r="E6" s="1">
+        <f>D6-C6</f>
+        <v>105000</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C9" s="1">
         <v>41745000</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="J10" s="1">
-        <f>J9*1.5%</f>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C10" s="1">
+        <f>C9*1.5%</f>
         <v>626175</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="I11" t="s">
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
         <v>14</v>
       </c>
-      <c r="J11" s="1">
-        <f>J9-J10</f>
+      <c r="C11" s="1">
+        <f>C9-C10</f>
         <v>41118825</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="I12" t="s">
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
         <v>15</v>
       </c>
-      <c r="J12" s="1">
+      <c r="C12" s="1">
         <f>3%*(41745000+4174500)</f>
         <v>1377585</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="I13" t="s">
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
         <v>16</v>
       </c>
-      <c r="J13" s="1">
-        <f>J11-J12</f>
+      <c r="C13" s="1">
+        <f>C11-C12</f>
         <v>39741240</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="I14" t="s">
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
         <v>17</v>
       </c>
-      <c r="J14" s="1">
-        <f>J13/110</f>
+      <c r="C14" s="1">
+        <f>C13/110</f>
         <v>361284</v>
       </c>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
krtik ukuran dp2nt16 dan dp1nt9
</commit_message>
<xml_diff>
--- a/Kaos/REKAPITULASI.xlsx
+++ b/Kaos/REKAPITULASI.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mapan\progress\Kaos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F903C6BA-5CA7-4C58-B867-13C72F6C9FAD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EF3E9FB-43D1-47A6-A5C8-B56647B1C179}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
   <si>
     <t>NO</t>
   </si>
@@ -37,9 +37,6 @@
     <t>TGL</t>
   </si>
   <si>
-    <t>BANYAK</t>
-  </si>
-  <si>
     <t>BAYAR</t>
   </si>
   <si>
@@ -86,6 +83,9 @@
   </si>
   <si>
     <t>24 MARET 2021</t>
+  </si>
+  <si>
+    <t>KIRIM</t>
   </si>
 </sst>
 </file>
@@ -418,10 +418,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L15"/>
+  <dimension ref="A1:L23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="216" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -446,16 +446,16 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
       <c r="F1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
         <v>9</v>
-      </c>
-      <c r="G1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -463,10 +463,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2">
         <v>120</v>
@@ -474,7 +474,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D3">
         <v>120</v>
@@ -482,7 +482,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D4">
         <v>120</v>
@@ -493,10 +493,10 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E6">
         <v>110</v>
@@ -532,7 +532,7 @@
         <v>44287</v>
       </c>
       <c r="C10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D10">
         <v>30</v>
@@ -543,7 +543,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D11">
         <v>30</v>
@@ -552,25 +552,21 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14">
         <v>4</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B14" s="3">
         <v>44289</v>
       </c>
-      <c r="C13" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13">
-        <v>70</v>
-      </c>
-      <c r="F13" s="1">
-        <f>F11+D13</f>
-        <v>110</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
         <v>6</v>
       </c>
@@ -578,18 +574,76 @@
         <v>70</v>
       </c>
       <c r="F14" s="1">
+        <f>F11+D14</f>
         <v>110</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D15">
         <v>70</v>
       </c>
       <c r="F15" s="1">
         <v>110</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16">
+        <v>70</v>
+      </c>
+      <c r="F16" s="1">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>5</v>
+      </c>
+      <c r="B18" s="3">
+        <v>44298</v>
+      </c>
+      <c r="C18" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18">
+        <v>120</v>
+      </c>
+      <c r="F18" s="1">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19">
+        <v>120</v>
+      </c>
+      <c r="F19" s="1">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20">
+        <v>120</v>
+      </c>
+      <c r="F20" s="1">
+        <f>F16+D20</f>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F23" s="1">
+        <f>350*350000</f>
+        <v>122500000</v>
       </c>
     </row>
   </sheetData>
@@ -612,19 +666,19 @@
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="E2" s="1"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" s="1">
         <v>155000</v>
@@ -636,7 +690,7 @@
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" s="1">
         <v>60000</v>
@@ -648,7 +702,7 @@
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5" s="1">
         <v>40000</v>
@@ -699,7 +753,7 @@
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C11" s="1">
         <f>C9-C10</f>
@@ -710,7 +764,7 @@
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C12" s="1">
         <f>3%*(41745000+4174500)</f>
@@ -721,7 +775,7 @@
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C13" s="1">
         <f>C11-C12</f>
@@ -732,7 +786,7 @@
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C14" s="1">
         <f>C13/110</f>

</xml_diff>

<commit_message>
kirim 70 set 06mei2021
</commit_message>
<xml_diff>
--- a/Kaos/REKAPITULASI.xlsx
+++ b/Kaos/REKAPITULASI.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mapan\progress\Kaos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{570FB249-1150-4877-B523-FA5F4832FDDF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D9A8062-CAF6-4AD0-88F1-5C730D630D1D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="21">
   <si>
     <t>NO</t>
   </si>
@@ -86,6 +86,9 @@
   </si>
   <si>
     <t>KIRIM</t>
+  </si>
+  <si>
+    <t>6 MEI</t>
   </si>
 </sst>
 </file>
@@ -418,10 +421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L27"/>
+  <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="216" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -683,10 +686,79 @@
         <v>410</v>
       </c>
     </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>7</v>
+      </c>
+      <c r="C26" t="s">
+        <v>17</v>
+      </c>
+      <c r="E26">
+        <v>410</v>
+      </c>
+      <c r="F26" s="1">
+        <f>F22-E26</f>
+        <v>0</v>
+      </c>
+    </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E27">
+        <v>410</v>
+      </c>
       <c r="F27" s="1">
-        <f>410*350000</f>
-        <v>143500000</v>
+        <f t="shared" ref="F27:F28" si="2">F23-E27</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E28">
+        <v>410</v>
+      </c>
+      <c r="F28" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>8</v>
+      </c>
+      <c r="B30" t="s">
+        <v>20</v>
+      </c>
+      <c r="C30" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30">
+        <v>70</v>
+      </c>
+      <c r="F30" s="1">
+        <f>F26+D30</f>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
+        <v>5</v>
+      </c>
+      <c r="D31">
+        <v>70</v>
+      </c>
+      <c r="F31" s="1">
+        <f t="shared" ref="F31:F32" si="3">F27+D31</f>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>7</v>
+      </c>
+      <c r="D32">
+        <v>70</v>
+      </c>
+      <c r="F32" s="1">
+        <f t="shared" si="3"/>
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cetak pdu beda warna
</commit_message>
<xml_diff>
--- a/Kaos/REKAPITULASI.xlsx
+++ b/Kaos/REKAPITULASI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mapan\progress\Kaos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D656939-F3E3-48FA-9610-0055CF1EDFBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0589D416-CCDC-47C9-B395-4478ECEF5A64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="38">
   <si>
     <t>NO</t>
   </si>
@@ -135,6 +135,12 @@
   </si>
   <si>
     <t xml:space="preserve"> 19 APRIL 2021</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>110 SET</t>
   </si>
 </sst>
 </file>
@@ -206,7 +212,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -226,9 +232,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -237,6 +240,12 @@
     </xf>
     <xf numFmtId="42" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -936,7 +945,7 @@
         <v>170</v>
       </c>
       <c r="F40" s="1">
-        <f t="shared" ref="F39:F40" si="5">F36-E40</f>
+        <f t="shared" ref="F40" si="5">F36-E40</f>
         <v>0</v>
       </c>
     </row>
@@ -1073,10 +1082,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C801C50D-43EE-4BA0-99C5-093CD08C00D4}">
-  <dimension ref="A2:E22"/>
+  <dimension ref="A2:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:E21"/>
+      <selection activeCell="A17" sqref="A17:E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
@@ -1246,71 +1255,88 @@
       <c r="A18" s="8">
         <v>1</v>
       </c>
-      <c r="B18" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="D18" s="11">
-        <v>10000</v>
-      </c>
-      <c r="E18" s="11">
-        <f>410*D18</f>
-        <v>4100000</v>
+      <c r="B18" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
         <v>2</v>
       </c>
-      <c r="B19" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="C19" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="D19" s="11">
+      <c r="B19" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D19" s="10">
         <v>10000</v>
       </c>
-      <c r="E19" s="11">
-        <f>170*D19</f>
-        <v>1700000</v>
+      <c r="E19" s="10">
+        <f>410*D19</f>
+        <v>4100000</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="8">
         <v>3</v>
       </c>
-      <c r="B20" s="10" t="s">
+      <c r="B20" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D20" s="10">
+        <v>10000</v>
+      </c>
+      <c r="E20" s="10">
+        <f>170*D20</f>
+        <v>1700000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="8">
+        <v>4</v>
+      </c>
+      <c r="B21" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C20" s="10" t="s">
+      <c r="C21" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="D20" s="11">
+      <c r="D21" s="10">
         <v>10000</v>
       </c>
-      <c r="E20" s="11">
-        <f>400*D20</f>
+      <c r="E21" s="10">
+        <f>400*D21</f>
         <v>4000000</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="8"/>
-      <c r="B21" s="10"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="12" t="s">
+    <row r="22" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="8"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="E21" s="12">
-        <f>SUM(E18:E20)</f>
+      <c r="E22" s="11">
+        <f>SUM(E19:E21)</f>
         <v>9800000</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>